<commit_message>
Updates to data files
Adding some math and graph changes.
</commit_message>
<xml_diff>
--- a/WatchDataFiles/2016-02-17-05.xlsx
+++ b/WatchDataFiles/2016-02-17-05.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="13300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="2016-02-17-05" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>micro</t>
+  </si>
+  <si>
+    <t>milli</t>
+  </si>
+  <si>
+    <t>1341 Samples</t>
+  </si>
+  <si>
+    <t>~56 samples per second</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24364,11 +24381,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2105043904"/>
-        <c:axId val="-2105046240"/>
+        <c:axId val="-2129467648"/>
+        <c:axId val="-2129464960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2105043904"/>
+        <c:axId val="-2129467648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24377,7 +24394,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105046240"/>
+        <c:crossAx val="-2129464960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24385,7 +24402,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2105046240"/>
+        <c:axId val="-2129464960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24396,7 +24413,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105043904"/>
+        <c:crossAx val="-2129467648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24716,15 +24733,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1341"/>
+  <dimension ref="A1:P1341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1314" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G1341"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1372250601976</v>
       </c>
@@ -24746,8 +24763,33 @@
       <c r="G1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I1">
+        <v>1372250601976</v>
+      </c>
+      <c r="J1">
+        <v>1372250842633</v>
+      </c>
+      <c r="K1">
+        <f>J1-I1</f>
+        <v>240657</v>
+      </c>
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1">
+        <v>0.24</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1">
+        <v>240</v>
+      </c>
+      <c r="P1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1372250602155</v>
       </c>
@@ -24769,8 +24811,21 @@
       <c r="G2">
         <v>4.1279000000000003E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>1372250601976</v>
+      </c>
+      <c r="J2">
+        <v>1372250712244</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:K3" si="0">J2-I2</f>
+        <v>110268</v>
+      </c>
+      <c r="O2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1372250602329</v>
       </c>
@@ -24792,8 +24847,18 @@
       <c r="G3">
         <v>4.3143210000000001E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>1372250712244</v>
+      </c>
+      <c r="J3">
+        <v>1372250842633</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>130389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1372250602508</v>
       </c>
@@ -24816,7 +24881,7 @@
         <v>6.3649549999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1372250602688</v>
       </c>
@@ -24839,7 +24904,7 @@
         <v>5.4328486000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1372250602867</v>
       </c>
@@ -24862,7 +24927,7 @@
         <v>4.8203215000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1372250603047</v>
       </c>
@@ -24885,7 +24950,7 @@
         <v>3.5952676000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1372250603226</v>
       </c>
@@ -24908,7 +24973,7 @@
         <v>5.0333745999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1372250603406</v>
       </c>
@@ -24931,7 +24996,7 @@
         <v>3.9947416999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1372250603586</v>
       </c>
@@ -24954,7 +25019,7 @@
         <v>5.0600063000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1372250603766</v>
       </c>
@@ -24977,7 +25042,7 @@
         <v>5.0600063000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1372250603946</v>
       </c>
@@ -25000,7 +25065,7 @@
         <v>4.527374E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1372250604124</v>
       </c>
@@ -25023,7 +25088,7 @@
         <v>5.0866376999999997E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1372250604306</v>
       </c>
@@ -25046,7 +25111,7 @@
         <v>5.0067430000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1372250604484</v>
       </c>
@@ -25069,7 +25134,7 @@
         <v>7.1372720000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1372250604665</v>
       </c>

</xml_diff>